<commit_message>
Alterei as descrições dos useCases e removi os userStories
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint4/Rafael Mira/Use_case_Descriptions.xlsx
+++ b/Project/Phase 2/Sprint4/Rafael Mira/Use_case_Descriptions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <r>
       <rPr>
@@ -104,40 +104,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhuma</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso foi adicionado ao projeto.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -223,40 +189,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir. O recurso tem que estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: As informações do recurso foram alteradas.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -342,40 +274,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir. O recurso tem que estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso foi eliminado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -461,40 +359,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir. O recurso tem que estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso foi copiado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -580,40 +444,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir. O recurso tem que estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso foi cortado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -699,40 +529,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Tem que haver um recurso previamente copiado ou recortado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso foi colado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -818,40 +614,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir. O recurso tem que estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O e-mail foi colado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -937,40 +699,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso está selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -1056,40 +784,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir. O recurso tem que estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador consulta as informações sobre o recurso.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -1175,40 +869,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O recurso tem que existir. O recurso tem que estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador tem a janela de propriedades do recurso aberta.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -1302,41 +962,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador tem a janela de propriedades do recurso aberta.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -1447,41 +1072,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">   O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O nome do recurso foi definido.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -1592,41 +1182,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O telefone do recurso foi definido.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -1737,41 +1292,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O e-mail do recurso foi definido.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -1882,41 +1402,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: A função do recurso foi definida.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -2021,41 +1506,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: A taxa de pagamento do recurso foi definida.</t>
-    </r>
-  </si>
-  <si>
     <t>################################################################################################################### Diagrama 2</t>
   </si>
   <si>
@@ -2150,41 +1600,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Os dias de folga foram adicionados ao recurso.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -2270,41 +1685,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Os dias de folga foram eliminados do recurso.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -2384,41 +1764,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Os dias de estão selecionados.</t>
-    </r>
-  </si>
-  <si>
     <t>################################################################################################################### Diagrama 3</t>
   </si>
   <si>
@@ -2513,41 +1858,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  O recurso pode não existir mas nesse caso, tem que estar a ser criado.
-                            Se o recurso já existe, então tem de estar selecionado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: As colunas foram adicionadas ao diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -2633,41 +1943,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  Tem que existir pelo menos um recurso e este tem que estar selecionado. 
-                            A coluna tem que estar selecionada.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: As colunas foram eliminadas do diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -2753,41 +2028,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  Tem que existir pelo menos um recurso e este tem que estar selecionado. 
-                            A coluna tem que estar selecionada. A coluna tem que estar visível.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: As colunas foram eliminadas do diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -2867,27 +2107,6 @@
     </r>
   </si>
   <si>
-    <t>Pré-condições:  Tem que existir pelo menos um recurso e este tem que estar selecionado. 
-                          A coluna tem que estar selecionada. A coluna tem que estar oculta.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: As colunas estão visíveis no diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -2979,41 +2198,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  Tem que existir pelo menos um recurso e este tem que estar selecionado. 
-                            A coluna tem que existir.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: A coluna está selecionada.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -3099,41 +2283,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pré-condições:</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">  Tem que existir pelo menos um recurso e este tem que estar selecionado. 
-                            A coluna tem que existir. A coluna tem que estar selecionada.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: A coluna está selecionada.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -3238,27 +2387,6 @@
     </r>
   </si>
   <si>
-    <t>Pré-condições:  Tem que existir pelo menos um recurso e este tem que estar selecionado. 
-                          A coluna tem que existir. A coluna tem que estar selecionada.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O nome da coluna foi alterado.</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -3375,23 +2503,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O valor da coluna foi alterado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -3502,23 +2613,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O tipo de dados da coluna foi alterado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>Nome</t>
     </r>
     <r>
@@ -3620,27 +2714,6 @@
         <color theme="1"/>
       </rPr>
       <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <t>Pré-condições:  Tem que existir pelo menos um recurso e este tem que estar selecionado. 
-                          A coluna tem que existir. A coluna tem que estar selecionada.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Pós-condições</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O tipo a visibilidade do valor da coluna foi alterada.</t>
     </r>
   </si>
 </sst>
@@ -3955,1049 +3028,763 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="17.25" customHeight="1">
-      <c r="D6" s="1" t="s">
+    <row r="6" ht="17.25" customHeight="1"/>
+    <row r="8">
+      <c r="D8" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="D7" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
       <c r="D18" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="D20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
       <c r="D22" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23">
       <c r="D23" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25">
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
       <c r="D26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="D27" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="D29" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30">
       <c r="D30" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="D32" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33">
       <c r="D33" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="D34" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36">
       <c r="D36" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37">
       <c r="D37" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39">
       <c r="D39" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="D41" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="D42" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="D40" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43">
       <c r="D43" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44">
       <c r="D44" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45">
       <c r="D45" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46">
       <c r="D46" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47">
       <c r="D47" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="D49" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50">
       <c r="D50" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51">
       <c r="D51" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52">
       <c r="D52" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53">
       <c r="D53" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54">
       <c r="D54" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="D55" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57">
       <c r="D57" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58">
       <c r="D58" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59">
       <c r="D59" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60">
       <c r="D60" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61">
       <c r="D61" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="D62" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="D63" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="D64" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="65">
       <c r="D65" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66">
       <c r="D66" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67">
       <c r="D67" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="68">
       <c r="D68" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="D69" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="D70" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71">
       <c r="D71" s="1" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="D72" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="73">
       <c r="D73" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74">
       <c r="D74" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75">
       <c r="D75" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="D76" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="D77" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78">
       <c r="D78" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79">
       <c r="D79" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="D80" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="81">
       <c r="D81" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82">
       <c r="D82" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83">
       <c r="D83" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="D84" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="D85" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86">
       <c r="D86" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87">
       <c r="D87" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="D88" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="89">
       <c r="D89" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90">
       <c r="D90" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91">
       <c r="D91" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="D92" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="D93" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="94">
       <c r="D94" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="95">
       <c r="D95" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96">
       <c r="D96" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="D97" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="98">
       <c r="D98" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99">
       <c r="D99" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="D100" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="D101" s="1" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="102">
       <c r="D102" s="1" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="103">
       <c r="D103" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104">
       <c r="D104" s="1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105">
       <c r="D105" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="D106" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="107">
       <c r="D107" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="D108" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="D109" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110">
       <c r="D110" s="1" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111">
       <c r="D111" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112">
       <c r="D112" s="1" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="113">
       <c r="D113" s="1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114">
       <c r="D114" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="D116" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="D117" s="1" t="s">
-        <v>102</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="D115" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="118">
-      <c r="D118" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="D119" s="1" t="s">
-        <v>104</v>
+      <c r="D118" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="120">
       <c r="D120" s="1" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121">
       <c r="D121" s="1" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="122">
       <c r="D122" s="1" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="123">
       <c r="D123" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="D125" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="D126" s="1" t="s">
-        <v>110</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="D124" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="127">
       <c r="D127" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128">
       <c r="D128" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="129">
       <c r="D129" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="130">
       <c r="D130" s="1" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="131">
       <c r="D131" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="D132" s="1" t="s">
-        <v>116</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="D134" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="135">
-      <c r="D135" s="4" t="s">
-        <v>117</v>
+      <c r="D135" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="D136" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="137">
       <c r="D137" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
     <row r="138">
       <c r="D138" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="D139" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="D140" s="1" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="141">
-      <c r="D141" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="D142" s="1" t="s">
-        <v>123</v>
+      <c r="D141" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="143">
-      <c r="D143" s="1" t="s">
-        <v>124</v>
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144">
+      <c r="D144" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="145">
       <c r="D145" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="146">
       <c r="D146" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="147">
       <c r="D147" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="148">
       <c r="D148" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="D149" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="D150" s="1" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
     <row r="151">
       <c r="D151" s="1" t="s">
-        <v>131</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="D152" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="153">
       <c r="D153" s="1" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="154">
       <c r="D154" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="155">
       <c r="D155" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="D156" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="D157" s="1" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
     </row>
     <row r="158">
       <c r="D158" s="1" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
     </row>
     <row r="159">
       <c r="D159" s="1" t="s">
-        <v>138</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="D160" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="161">
-      <c r="D161" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="D163" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="D164" s="1" t="s">
-        <v>141</v>
+      <c r="D161" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="D162" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="165">
       <c r="D165" s="1" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
     </row>
     <row r="166">
       <c r="D166" s="1" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
     </row>
     <row r="167">
       <c r="D167" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
     </row>
     <row r="168">
       <c r="D168" s="1" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
     </row>
     <row r="169">
       <c r="D169" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="D171" s="1" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
     </row>
     <row r="172">
       <c r="D172" s="1" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
     </row>
     <row r="173">
       <c r="D173" s="1" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
     </row>
     <row r="174">
       <c r="D174" s="1" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
     </row>
     <row r="175">
       <c r="D175" s="1" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
     </row>
     <row r="176">
       <c r="D176" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="D177" s="1" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
     </row>
     <row r="179">
       <c r="D179" s="1" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
     </row>
     <row r="180">
       <c r="D180" s="1" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
     </row>
     <row r="181">
       <c r="D181" s="1" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
     </row>
     <row r="182">
       <c r="D182" s="1" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
     </row>
     <row r="183">
       <c r="D183" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="D184" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="D185" s="1" t="s">
-        <v>160</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="D186" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="187">
       <c r="D187" s="1" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="188">
       <c r="D188" s="1" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="189">
       <c r="D189" s="1" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
     </row>
     <row r="190">
       <c r="D190" s="1" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
     </row>
     <row r="191">
       <c r="D191" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="D192" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="D193" s="1" t="s">
-        <v>167</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="D194" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="195">
       <c r="D195" s="1" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
     </row>
     <row r="196">
       <c r="D196" s="1" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
     </row>
     <row r="197">
       <c r="D197" s="1" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
     </row>
     <row r="198">
       <c r="D198" s="1" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
     </row>
     <row r="199">
       <c r="D199" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="D200" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="D201" s="1" t="s">
-        <v>174</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="D202" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="203">
       <c r="D203" s="1" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="204">
       <c r="D204" s="1" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
     </row>
     <row r="205">
       <c r="D205" s="1" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
     </row>
     <row r="206">
       <c r="D206" s="1" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
     </row>
     <row r="207">
       <c r="D207" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="D208" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="D209" s="1" t="s">
-        <v>181</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="D210" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="211">
       <c r="D211" s="1" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
     </row>
     <row r="212">
       <c r="D212" s="1" t="s">
-        <v>183</v>
+        <v>152</v>
       </c>
     </row>
     <row r="213">
       <c r="D213" s="1" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
     </row>
     <row r="214">
       <c r="D214" s="1" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
     </row>
     <row r="215">
       <c r="D215" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="D216" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="D217" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="D218" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="D220" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="D221" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="D222" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="D223" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="D224" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="D225" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="D226" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="D227" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="D229" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="D230" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="D231" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="D232" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="D233" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="D234" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="D235" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="D236" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="D238" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="D239" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="D240" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="D241" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="D242" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="D243" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="D244" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="D245" s="1" t="s">
-        <v>211</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizei os ids dos use cases v2.
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint4/Rafael Mira/Use_case_Descriptions.xlsx
+++ b/Project/Phase 2/Sprint4/Rafael Mira/Use_case_Descriptions.xlsx
@@ -43,7 +43,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 1</t>
+      <t>: 14</t>
     </r>
   </si>
   <si>
@@ -111,7 +111,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Alterar informação</t>
+      <t>: Alterar dados</t>
     </r>
   </si>
   <si>
@@ -128,7 +128,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 2</t>
+      <t>: 15</t>
     </r>
   </si>
   <si>
@@ -145,7 +145,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador altera as informações de um recurso do projeto.</t>
+      <t>: O utilizador altera dados do recurso.</t>
     </r>
   </si>
   <si>
@@ -213,7 +213,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 3</t>
+      <t>: 16</t>
     </r>
   </si>
   <si>
@@ -298,7 +298,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 4</t>
+      <t>: 17</t>
     </r>
   </si>
   <si>
@@ -383,7 +383,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 5</t>
+      <t>: 18</t>
     </r>
   </si>
   <si>
@@ -468,7 +468,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 6</t>
+      <t>: 19</t>
     </r>
   </si>
   <si>
@@ -553,7 +553,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 7</t>
+      <t>: 20</t>
     </r>
   </si>
   <si>
@@ -638,7 +638,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 8</t>
+      <t>: 21</t>
     </r>
   </si>
   <si>
@@ -706,7 +706,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Consultar informações</t>
+      <t>: Consultar dados</t>
     </r>
   </si>
   <si>
@@ -723,7 +723,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 9</t>
+      <t>: 22</t>
     </r>
   </si>
   <si>
@@ -740,7 +740,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador consulta informações sobre o recurso.</t>
+      <t>: O utilizador consulta dados sobre o recurso.</t>
     </r>
   </si>
   <si>
@@ -791,7 +791,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Mostrar propriedades do Recurso</t>
+      <t>: Aceder às propriedades do Recurso</t>
     </r>
   </si>
   <si>
@@ -808,7 +808,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 10</t>
+      <t>: 23</t>
     </r>
   </si>
   <si>
@@ -884,6 +884,150 @@
         <i/>
         <color theme="1"/>
       </rPr>
+      <t>Definir dados</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador define informação geral do recurso.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Definir Nome</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador define o nome do recurso.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Especializa</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
       <t>Definir informação geral</t>
     </r>
   </si>
@@ -894,6 +1038,57 @@
         <b/>
         <color theme="1"/>
       </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Definir Telefone</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
       <t>ID</t>
     </r>
     <r>
@@ -901,7 +1096,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 11</t>
+      <t>: 26</t>
     </r>
   </si>
   <si>
@@ -918,7 +1113,32 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador define informação geral do recurso.</t>
+      <t>: O utilizador define o telefone do recurso.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Especializa</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>Definir informação geral</t>
     </r>
   </si>
   <si>
@@ -969,7 +1189,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Definir Nome</t>
+      <t>: Definir E-mail</t>
     </r>
   </si>
   <si>
@@ -986,7 +1206,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 12</t>
+      <t>: 27</t>
     </r>
   </si>
   <si>
@@ -1003,7 +1223,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador define o nome do recurso.</t>
+      <t>: O utilizador define o e-mail do recurso.</t>
     </r>
   </si>
   <si>
@@ -1079,7 +1299,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Definir Telefone</t>
+      <t>: Definir Função</t>
     </r>
   </si>
   <si>
@@ -1096,7 +1316,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 13</t>
+      <t>: 28</t>
     </r>
   </si>
   <si>
@@ -1113,7 +1333,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador define o telefone do recurso.</t>
+      <t>: O utilizador define a função do recurso.</t>
     </r>
   </si>
   <si>
@@ -1189,7 +1409,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Definir E-mail</t>
+      <t>: Definir Taxa de pagamento</t>
     </r>
   </si>
   <si>
@@ -1206,7 +1426,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 14</t>
+      <t>: 29</t>
     </r>
   </si>
   <si>
@@ -1223,7 +1443,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador define o e-mail do recurso.</t>
+      <t>: O utilizador define a taxa de pagamento do recurso.</t>
     </r>
   </si>
   <si>
@@ -1286,6 +1506,9 @@
     </r>
   </si>
   <si>
+    <t>################################################################################################################### Diagrama 2</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1299,7 +1522,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Definir Função</t>
+      <t>: Adicionar folga</t>
     </r>
   </si>
   <si>
@@ -1316,7 +1539,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 15</t>
+      <t>: 30</t>
     </r>
   </si>
   <si>
@@ -1333,7 +1556,775 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador define a função do recurso.</t>
+      <t>: O utilizador adiciona dias de folga ao recurso.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Eliminar folga</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador elimina dias de folga do recurso.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Selecionar Dias</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 32</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador seleciona os dias que quer adicionar ou eliminar do recurso.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <t>################################################################################################################### Diagrama 3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Adicionar coluna</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 33</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador adiciona colunas ao diagrama de recursos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Eliminar coluna</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador elimina colunas do diagrama de recursos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Ocultar coluna</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 35</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador oculta colunas do diagrama de recursos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Mostrar coluna</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 36</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador torna visíveis colunas do diagrama de recursos.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Selecionar coluna</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 37</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador selecionar uma coluna.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Alterar dados da coluna</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 38</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador altera dados da coluna.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ator Principal</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Utilizador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Atores Secundários</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Nenhum</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Nome</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: Alterar Nome</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: 39</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Descrição</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>: O utilizador altera o nome da coluna.</t>
     </r>
   </si>
   <si>
@@ -1358,7 +2349,7 @@
         <i/>
         <color theme="1"/>
       </rPr>
-      <t>Definir informação geral</t>
+      <t>Alterar dados da coluna</t>
     </r>
   </si>
   <si>
@@ -1409,7 +2400,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Definir Taxa de pagamento</t>
+      <t>: Alterar valor</t>
     </r>
   </si>
   <si>
@@ -1426,7 +2417,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 16</t>
+      <t>: 40</t>
     </r>
   </si>
   <si>
@@ -1443,7 +2434,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador define a taxa de pagamento do recurso.</t>
+      <t>: O utilizador altera o valor da coluna.</t>
     </r>
   </si>
   <si>
@@ -1468,7 +2459,7 @@
         <i/>
         <color theme="1"/>
       </rPr>
-      <t>Definir informação geral</t>
+      <t>Alterar dados da coluna</t>
     </r>
   </si>
   <si>
@@ -1506,9 +2497,6 @@
     </r>
   </si>
   <si>
-    <t>################################################################################################################### Diagrama 2</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1522,7 +2510,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Adicionar folga</t>
+      <t>: Alterar tipo de dados</t>
     </r>
   </si>
   <si>
@@ -1539,7 +2527,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 17</t>
+      <t>: 41</t>
     </r>
   </si>
   <si>
@@ -1556,7 +2544,32 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: O utilizador adiciona dias de folga ao recurso.</t>
+      <t>: O utilizador altera o tipo de dados da coluna.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Especializa</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>Alterar dados da coluna</t>
     </r>
   </si>
   <si>
@@ -1607,7 +2620,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: Eliminar folga</t>
+      <t>: Alterar visibilidade do valor</t>
     </r>
   </si>
   <si>
@@ -1624,1020 +2637,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>: 18</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador elimina dias de folga do recurso.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Selecionar Dias</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador seleciona os dias que quer adicionar ou eliminar do recurso.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <t>################################################################################################################### Diagrama 3</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Adicionar coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador adiciona colunas ao diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Eliminar coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 21</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador elimina colunas do diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Ocultar coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 22</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador oculta colunas do diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Mostrar coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 23</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador torna visíveis colunas do diagrama de recursos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Selecionar coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador selecionar uma coluna.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Alterar dados da coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador altera dados da coluna.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Alterar Nome</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador altera o nome da coluna.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Especializa</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>Alterar dados da coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Alterar valor</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador altera o valor da coluna.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Especializa</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>Alterar dados da coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Alterar tipo de dados</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 28</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Descrição</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: O utilizador altera o tipo de dados da coluna.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Especializa</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>Alterar dados da coluna</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Ator Principal</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Utilizador</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Atores Secundários</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Nenhum</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Nome</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: Alterar visibilidade do valor</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>: 28</t>
+      <t>: 42</t>
     </r>
   </si>
   <si>

</xml_diff>